<commit_message>
Corrección Universitat Jaume I y agregar entrara par académico (+ links a cada revista)
</commit_message>
<xml_diff>
--- a/data/educacion.xlsx
+++ b/data/educacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanl\Desktop\Moni_HV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Moni_HV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863E5D7B-3342-433F-94FE-DF6105325AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615C600-8352-42CF-BBBE-464E96A500A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -67,13 +67,13 @@
     <t xml:space="preserve">Maestría en Igualdad de género en ámbito público y privado </t>
   </si>
   <si>
-    <t>Universidad Jaime I</t>
-  </si>
-  <si>
     <t>Doctorado en Investigación de Medios de Comunicación</t>
   </si>
   <si>
     <t>Castellón de la Plana, España</t>
+  </si>
+  <si>
+    <t>Universitat Jaume I</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -968,10 +968,10 @@
         <v>2017</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mejorar formato de trabajos de grado dirigidos (agregando siempre el argumento '.protect = FALSE' a la función 'detailed_entries' para poder agregar formato en LaTeX e hipervínculos)
</commit_message>
<xml_diff>
--- a/data/educacion.xlsx
+++ b/data/educacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Moni_HV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615C600-8352-42CF-BBBE-464E96A500A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6155734D-6D42-4E50-A9D0-AD23B7319325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>what</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Universitat Jaume I</t>
+  </si>
+  <si>
+    <t>Tesis: \href{http://hdl.handle.net/10234/167275}{Implementar una guía para el seguimiento periodístico con enfoque de género de las desmovilizaciones de las FARC}</t>
+  </si>
+  <si>
+    <t>Tesis: \href{http://hdl.handle.net/10016/35862}{El tratamiento periodístico de la violencia sexual en contra de las mujeres en el marco del conflicto armado colombiano. Análisis de casos según el tipo de violencia, víctimas, victimarios y contextos}. \textit{Cum Laude} y mención Internacional</t>
   </si>
 </sst>
 </file>
@@ -557,8 +563,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -917,7 +926,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -959,8 +968,11 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -972,6 +984,9 @@
       </c>
       <c r="D3" t="s">
         <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>